<commit_message>
update 27 februari 2023
</commit_message>
<xml_diff>
--- a/Fazzprint/Project/Watermark Undangan.xlsx
+++ b/Fazzprint/Project/Watermark Undangan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Habibullah\Documents\Fazzprint\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9754D7-77AD-4E0E-AF66-1AEE2BD0EDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,7 +77,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -83,6 +89,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -131,7 +140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,9 +173,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,6 +225,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -374,17 +417,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B34:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.7109375" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.73046875" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="27.7109375" style="1"/>
+    <col min="1" max="16384" width="27.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="34" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
@@ -400,7 +443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
         <v>2</v>
       </c>
@@ -408,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
@@ -418,29 +461,29 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="142" scale="98" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="126" scale="98" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>